<commit_message>
just a small change
</commit_message>
<xml_diff>
--- a/Maths DS.xlsx
+++ b/Maths DS.xlsx
@@ -370,21 +370,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O75" sqref="O75"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>